<commit_message>
minor param dist updates
</commit_message>
<xml_diff>
--- a/biorefineries/succinic/analyses/parameter_distributions/parameter-distributions_lab-scale_batch.xlsx
+++ b/biorefineries/succinic/analyses/parameter_distributions/parameter-distributions_lab-scale_batch.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\succinic\analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\succinic\analyses\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCDB166-013C-45B5-BBD1-9D8691F433C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4A1A78-400A-412C-A07B-F71D26579C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -438,8 +438,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -722,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,7 +737,7 @@
     <col min="11" max="11" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -773,7 +772,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -804,7 +803,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -835,7 +834,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -868,7 +867,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -901,7 +900,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -934,7 +933,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -967,7 +966,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>66</v>
       </c>
@@ -1033,7 +1032,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>69</v>
       </c>
@@ -1066,7 +1065,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>71</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>72</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>83</v>
       </c>
@@ -1261,14 +1260,9 @@
       <c r="K16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1280,22 +1274,22 @@
       <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <f>(0.345+0.357)/2</f>
         <v>0.35099999999999998</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <f>0.8*E17</f>
         <v>0.28079999999999999</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <f>E17</f>
         <v>0.35099999999999998</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <f>1.2*E17</f>
         <v>0.42119999999999996</v>
       </c>
@@ -1303,14 +1297,9 @@
       <c r="K17" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-    </row>
-    <row r="18" spans="1:18" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    </row>
+    <row r="18" spans="1:14" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1322,22 +1311,22 @@
       <c r="D18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <f>(45.97+47.63)/2</f>
         <v>46.8</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <f>0.8*E18</f>
         <v>37.44</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <f>E18</f>
         <v>46.8</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <f>1.2*E18</f>
         <v>56.16</v>
       </c>
@@ -1345,14 +1334,10 @@
       <c r="K18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1364,18 +1349,18 @@
       <c r="D19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f>(0.661+0.968)/2</f>
         <v>0.8145</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>0.66100000000000003</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6">
         <v>0.96799999999999997</v>
       </c>
       <c r="J19" s="3"/>
@@ -1383,7 +1368,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1419,7 +1404,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>85</v>
       </c>
@@ -1451,7 +1436,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>73</v>
       </c>
@@ -1485,7 +1470,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>74</v>
       </c>
@@ -1518,7 +1503,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>75</v>
       </c>
@@ -1550,7 +1535,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>88</v>
       </c>
@@ -1582,7 +1567,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -1615,7 +1600,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1650,7 +1635,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -1683,7 +1668,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
attribute uncertainty to fermentation power utility
</commit_message>
<xml_diff>
--- a/biorefineries/succinic/analyses/parameter_distributions/parameter-distributions_lab-scale_batch.xlsx
+++ b/biorefineries/succinic/analyses/parameter_distributions/parameter-distributions_lab-scale_batch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\succinic\analyses\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4A1A78-400A-412C-A07B-F71D26579C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6D0EF5-1E90-4421-BE77-66F6668FBCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="94">
   <si>
     <t>Parameter name</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t>Triangular</t>
+  </si>
+  <si>
+    <t>Fermentation kW per m3</t>
+  </si>
+  <si>
+    <t>R302.kW_per_m3 = x</t>
+  </si>
+  <si>
+    <t>kW/m3</t>
   </si>
 </sst>
 </file>
@@ -401,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -424,11 +433,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,6 +461,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,41 +1590,41 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>34</v>
+      <c r="A26" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3" t="s">
-        <v>59</v>
+        <v>93</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0.19885</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="9">
+        <f>0.8*E26</f>
+        <v>0.15908</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9">
+        <f>1.2*E26</f>
+        <v>0.23862</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>18</v>
@@ -1614,88 +1636,121 @@
         <v>17</v>
       </c>
       <c r="E27" s="3">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>90</v>
       </c>
       <c r="G27" s="3">
-        <f>0.8*E27</f>
-        <v>0.68</v>
+        <v>0.8</v>
       </c>
       <c r="H27" s="3">
-        <f>E27</f>
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="I27" s="3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E28" s="3">
-        <v>168</v>
+        <v>0.85</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>90</v>
       </c>
       <c r="G28" s="3">
-        <v>134.4</v>
+        <f>0.8*E28</f>
+        <v>0.68</v>
       </c>
       <c r="H28" s="3">
-        <v>168</v>
+        <f>E28</f>
+        <v>0.85</v>
       </c>
       <c r="I28" s="3">
-        <v>201.6</v>
+        <v>1</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E29" s="3">
-        <v>0.8</v>
+        <v>168</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="G29" s="3">
-        <v>0.72000000000000008</v>
-      </c>
-      <c r="H29" s="3"/>
+        <v>134.4</v>
+      </c>
+      <c r="H29" s="3">
+        <v>168</v>
+      </c>
       <c r="I29" s="3">
-        <v>0.88000000000000012</v>
+        <v>201.6</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.72000000000000008</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3">
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>